<commit_message>
Mise à jour fichier tâches
</commit_message>
<xml_diff>
--- a/doc/taches.xlsx
+++ b/doc/taches.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Création de layout</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Controller Pages</t>
   </si>
   <si>
-    <t>Vue home</t>
-  </si>
-  <si>
     <t>Vue show</t>
   </si>
   <si>
@@ -105,12 +102,6 @@
     <t>Permet de modifier les users</t>
   </si>
   <si>
-    <t>Après un login ok</t>
-  </si>
-  <si>
-    <t>Suite à un problème de login</t>
-  </si>
-  <si>
     <t>Vue mentionslegales</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
   </si>
   <si>
     <t>Controller Disciplines</t>
-  </si>
-  <si>
-    <t>Menu principal après login</t>
   </si>
   <si>
     <t xml:space="preserve">Pour gérer les infos des licencies </t>
@@ -234,12 +222,21 @@
   <si>
     <t>Vue index</t>
   </si>
+  <si>
+    <t>pdf + csv</t>
+  </si>
+  <si>
+    <t>Après un register ok</t>
+  </si>
+  <si>
+    <t>Suite à un problème de register</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,19 +296,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -321,19 +305,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -396,7 +367,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -427,20 +398,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -804,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -820,11 +781,11 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="5"/>
@@ -836,266 +797,304 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30">
-      <c r="B7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30">
-      <c r="A12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>42</v>
+      <c r="D14" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
       <c r="A19" s="11"/>
-      <c r="B19" s="17" t="s">
-        <v>18</v>
+      <c r="B19" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30">
       <c r="B30" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="1"/>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>42</v>
+      <c r="A33" s="10"/>
+      <c r="B33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="1"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
+      <c r="A36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1103,135 +1102,104 @@
         <v>20</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1"/>
-      <c r="B45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="4" t="s">
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="7" t="s">
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="4" t="s">
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="B61" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>